<commit_message>
Fix in the template columns
</commit_message>
<xml_diff>
--- a/reports/approved_requests/templates/template.xlsx
+++ b/reports/approved_requests/templates/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\global-connect-reports\reports\approved_requests\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D4726D-1689-440C-9DA2-100A302B3B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4F4F7-74FE-4572-828B-E23A599C49AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,72 +16,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AL$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Anastasia Tsyrendorzhieva</author>
-  </authors>
-  <commentList>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Anastasia Tsyrendorzhieva:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-New Billing Date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Anastasia Tsyrendorzhieva:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Subcription - Fullfilment - Request - Parameters -- can be different emails inside</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Request ID</t>
   </si>
@@ -140,9 +82,6 @@
     <t>Subscription Status</t>
   </si>
   <si>
-    <t>Anniversary Date</t>
-  </si>
-  <si>
     <t>Effective Date</t>
   </si>
   <si>
@@ -153,15 +92,6 @@
   </si>
   <si>
     <t>Currency</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Reseller Cost</t>
-  </si>
-  <si>
-    <t>MSRP</t>
   </si>
   <si>
     <t>Connection Type</t>
@@ -201,32 +131,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -270,12 +181,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,54 +493,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.08984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="27.1796875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="29.6328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="24.08984375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="4"/>
-    <col min="15" max="16" width="15.90625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="21" style="4" customWidth="1"/>
-    <col min="18" max="18" width="22.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="15.7265625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="14.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="18.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.08984375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="27.1796875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="29.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="24.08984375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" style="3"/>
+    <col min="15" max="16" width="15.90625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="21" style="3" customWidth="1"/>
+    <col min="18" max="18" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="15.7265625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="14.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,16 +548,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -679,13 +581,13 @@
         <v>10</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>12</v>
@@ -700,10 +602,10 @@
         <v>15</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>16</v>
@@ -714,7 +616,7 @@
       <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AC1" s="1" t="s">
@@ -723,35 +625,22 @@
       <c r="AD1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add temporal changes on templates.
</commit_message>
<xml_diff>
--- a/reports/approved_requests/templates/template.xlsx
+++ b/reports/approved_requests/templates/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\global-connect-reports\reports\approved_requests\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4F4F7-74FE-4572-828B-E23A599C49AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0632D4A8-1C50-420E-9057-F7D796EE8623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Request ID</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Customer Tenant Value</t>
+  </si>
+  <si>
+    <t>Reseller ID #</t>
+  </si>
+  <si>
+    <t>Vendor ID</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
   </si>
 </sst>
 </file>
@@ -494,9 +503,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -514,27 +525,29 @@
     <col min="12" max="12" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7265625" style="3"/>
-    <col min="15" max="16" width="15.90625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="21" style="3" customWidth="1"/>
-    <col min="18" max="18" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="15.7265625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="14.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.7265625" style="3"/>
+    <col min="15" max="15" width="15.90625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="18.6328125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="21" style="3" customWidth="1"/>
+    <col min="19" max="19" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="15.7265625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="14.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,62 +597,71 @@
         <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AK1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>